<commit_message>
database + error + filename upload
</commit_message>
<xml_diff>
--- a/Template/Test.xlsx
+++ b/Template/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="1326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="1327">
   <si>
     <t xml:space="preserve">Project ID(s)</t>
   </si>
@@ -3382,6 +3382,9 @@
   </si>
   <si>
     <t xml:space="preserve">FileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a.xlxs</t>
   </si>
   <si>
     <t xml:space="preserve">Strategy ID(s)</t>
@@ -4108,9 +4111,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.984693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,14 +4502,13 @@
   </sheetPr>
   <dimension ref="A1:ALM9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7597,7 +7598,7 @@
         <v>1119</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>104</v>
+        <v>1120</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>1112</v>
@@ -7621,645 +7622,644 @@
   </sheetPr>
   <dimension ref="A1:GY8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="BX1" s="0" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="BZ1" s="0" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="CC1" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="CD1" s="0" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="CE1" s="0" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="CF1" s="0" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="CG1" s="0" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="CH1" s="0" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="CI1" s="0" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="CJ1" s="0" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="CK1" s="0" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="CL1" s="0" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="CM1" s="0" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="CN1" s="0" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="CO1" s="0" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="CP1" s="0" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="CQ1" s="0" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="CR1" s="0" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="CS1" s="0" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="CT1" s="0" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="CU1" s="0" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="CV1" s="0" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="CW1" s="0" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="CX1" s="0" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="CY1" s="0" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="CZ1" s="0" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="DA1" s="0" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="DB1" s="0" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="DC1" s="0" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="DD1" s="0" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="DE1" s="0" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="DF1" s="0" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="DG1" s="0" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="DH1" s="0" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="DI1" s="0" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="DJ1" s="0" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="DK1" s="0" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="DL1" s="0" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="DM1" s="0" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="DN1" s="0" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="DO1" s="0" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="DP1" s="0" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="DQ1" s="0" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="DR1" s="0" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="DS1" s="0" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="DT1" s="0" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="DU1" s="0" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="DV1" s="0" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="DW1" s="0" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="DX1" s="0" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="DY1" s="0" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="DZ1" s="0" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="EA1" s="0" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="EB1" s="0" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="EC1" s="0" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="ED1" s="0" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="EE1" s="0" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="EF1" s="0" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="EG1" s="0" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="EH1" s="0" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="EI1" s="0" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="EJ1" s="0" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="EK1" s="0" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="EL1" s="0" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="EM1" s="0" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="EN1" s="0" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="EO1" s="0" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="EP1" s="0" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="EQ1" s="0" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="ER1" s="0" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="ES1" s="0" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="ET1" s="0" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="EU1" s="0" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="EV1" s="0" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="EW1" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="EX1" s="0" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="EY1" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="EZ1" s="0" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="FA1" s="0" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="FB1" s="0" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="FC1" s="0" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="FD1" s="0" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="FE1" s="0" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="FF1" s="0" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="FG1" s="0" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="FH1" s="0" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="FI1" s="0" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="FJ1" s="0" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="FK1" s="0" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="FL1" s="0" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="FM1" s="0" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="FN1" s="0" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="FO1" s="0" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="FP1" s="0" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="FQ1" s="0" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="FR1" s="0" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="FS1" s="0" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="FT1" s="0" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="FU1" s="0" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="FV1" s="0" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="FW1" s="0" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="FX1" s="0" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="FY1" s="0" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="FZ1" s="0" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="GA1" s="0" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="GB1" s="0" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="GC1" s="0" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="GD1" s="0" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="GE1" s="0" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="GF1" s="0" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="GG1" s="0" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="GH1" s="0" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="GI1" s="0" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="GJ1" s="0" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="GK1" s="0" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="GL1" s="0" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="GM1" s="0" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="GN1" s="0" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="GO1" s="0" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="GP1" s="0" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="GQ1" s="0" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="GR1" s="0" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="GS1" s="0" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="GT1" s="0" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="GU1" s="0" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="GV1" s="0" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="GW1" s="0" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="GX1" s="0" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="GY1" s="0" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>1</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>112</v>
@@ -8275,7 +8275,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>113</v>
@@ -8291,7 +8291,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>104</v>
@@ -8299,7 +8299,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>104</v>

</xml_diff>